<commit_message>
Fibonacci e apresentação sprin 1
</commit_message>
<xml_diff>
--- a/Documentação/xlxs/Product Backlog.xlsx
+++ b/Documentação/xlxs/Product Backlog.xlsx
@@ -1,31 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINDOWS10\Desktop\BandTec\Pesquisa e Inovação\HealthServer\HealthServer\Documentação\xlxs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F24D21E-D95B-4855-9025-C98D5B347E2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19416" windowHeight="11016" tabRatio="885"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBC" sheetId="15" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="16" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t>Importante</t>
   </si>
@@ -156,24 +152,6 @@
     <t>Pontuação</t>
   </si>
   <si>
-    <t>Dylan</t>
-  </si>
-  <si>
-    <t>Arthur</t>
-  </si>
-  <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>Gabriel</t>
-  </si>
-  <si>
-    <t>Matheus</t>
-  </si>
-  <si>
-    <t>Felipe</t>
-  </si>
-  <si>
     <t>Fácil</t>
   </si>
   <si>
@@ -187,31 +165,16 @@
   </si>
   <si>
     <t>Muito Dificil</t>
-  </si>
-  <si>
-    <t>Tudo o que está com pontuação 3, é porque acredito que seja facil e há entendimento da minha parte.</t>
-  </si>
-  <si>
-    <t>Tudo o que está com pontuação 5, há entendimento da minha parte porem exige um pouco mais de tempo para desenvolver e maior contexto por trás.</t>
-  </si>
-  <si>
-    <t>Tudo o que está com pontuação 8, há entendimento da minha parte, mas exige tempo para desenvolvimento.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tudo o que está com pontuação 13, há entendimento da minha parte, porem, o desenvolvimento do mesmo exige mais estudo e entendimento dos valores </t>
-  </si>
-  <si>
-    <t>Pontuação: DYLAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -326,6 +289,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <name val="Exo"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="28"/>
+      <name val="Exo"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -383,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -556,6 +530,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -581,7 +611,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -618,9 +648,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,9 +663,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,23 +674,8 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -685,10 +694,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -696,6 +701,39 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -705,43 +743,88 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
@@ -1369,7 +1452,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1C237F12-9C79-4455-B9B4-0B3C619348CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C237F12-9C79-4455-B9B4-0B3C619348CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1432,7 +1515,7 @@
         <xdr:cNvPr id="5" name="Imagem 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{07C3E689-C90D-474C-A0DF-E823DF93503E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07C3E689-C90D-474C-A0DF-E823DF93503E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1782,11 +1865,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:T50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1"/>
@@ -1795,29 +1878,37 @@
     <col min="2" max="2" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="107" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="8.88671875" style="1"/>
-    <col min="11" max="11" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="9.77734375" style="58" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="1"/>
+    <col min="11" max="12" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="1"/>
+    <col min="16" max="16" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="1"/>
+    <col min="18" max="18" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="1"/>
+    <col min="20" max="20" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="19.5" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:20" ht="89.25" customHeight="1" thickBot="1">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="38"/>
-      <c r="N2" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42"/>
+      <c r="O2" s="5"/>
     </row>
     <row r="3" spans="2:20" ht="9.9" customHeight="1" thickBot="1"/>
     <row r="4" spans="2:20" s="5" customFormat="1" ht="24.9" customHeight="1" thickBot="1">
@@ -1830,609 +1921,768 @@
       <c r="D4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20" t="s">
+      <c r="E5" s="59">
+        <v>3</v>
+      </c>
+      <c r="F5" s="54"/>
+      <c r="G5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="K5" s="6">
+      <c r="H5" s="18"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+    </row>
+    <row r="6" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="60">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B6" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="K6" s="6">
+      <c r="F6" s="54"/>
+      <c r="G6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
+    </row>
+    <row r="7" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="60">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B7" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="K7" s="6">
+      <c r="F7" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
+      <c r="R7" s="65"/>
+      <c r="S7" s="65"/>
+      <c r="T7" s="65"/>
+    </row>
+    <row r="8" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="60">
+        <v>13</v>
+      </c>
+      <c r="F8" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="65"/>
+      <c r="S8" s="65"/>
+      <c r="T8" s="65"/>
+    </row>
+    <row r="9" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="61">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B8" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="K8" s="6">
+      <c r="F9" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="23"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="65"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="65"/>
+    </row>
+    <row r="10" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="56">
+        <v>13</v>
+      </c>
+      <c r="F10" s="54"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
+      <c r="N10" s="65"/>
+      <c r="O10" s="65"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
+    </row>
+    <row r="11" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="60">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B9" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="29"/>
-      <c r="K9" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B10" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="K10" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B11" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="F11" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
       <c r="I11" s="7"/>
       <c r="J11"/>
-      <c r="K11" s="7">
+      <c r="K11" s="66"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="65"/>
+      <c r="S11" s="65"/>
+      <c r="T11" s="65"/>
+    </row>
+    <row r="12" spans="2:20" s="6" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+      <c r="B12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="60">
+        <v>5</v>
+      </c>
+      <c r="F12" s="54"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="65"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="65"/>
+      <c r="S12" s="65"/>
+      <c r="T12" s="65"/>
+    </row>
+    <row r="13" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="62">
+        <v>3</v>
+      </c>
+      <c r="F13" s="54"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="65"/>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="65"/>
+      <c r="S13" s="65"/>
+      <c r="T13" s="65"/>
+    </row>
+    <row r="14" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="60">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="2:20" s="6" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="B12" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="K12" s="6">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B13" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="K13" s="6">
+      <c r="F14" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="65"/>
+      <c r="S14" s="65"/>
+      <c r="T14" s="65"/>
+    </row>
+    <row r="15" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="60">
+        <v>5</v>
+      </c>
+      <c r="F15" s="54"/>
+      <c r="G15" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="18"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="65"/>
+      <c r="O15" s="65"/>
+      <c r="P15" s="65"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="65"/>
+      <c r="S15" s="65"/>
+      <c r="T15" s="65"/>
+    </row>
+    <row r="16" spans="2:20" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="60">
+        <v>5</v>
+      </c>
+      <c r="F16" s="54"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="67"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
+      <c r="N16" s="65"/>
+      <c r="O16" s="65"/>
+      <c r="P16" s="65"/>
+      <c r="Q16" s="65"/>
+      <c r="R16" s="65"/>
+      <c r="S16" s="65"/>
+      <c r="T16" s="65"/>
+    </row>
+    <row r="17" spans="2:20" s="6" customFormat="1" ht="27" customHeight="1" thickBot="1">
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="60">
+        <v>5</v>
+      </c>
+      <c r="F17" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="65"/>
+      <c r="N17" s="65"/>
+      <c r="O17" s="65"/>
+      <c r="P17" s="65"/>
+      <c r="Q17" s="65"/>
+      <c r="R17" s="65"/>
+      <c r="S17" s="65"/>
+      <c r="T17" s="65"/>
+    </row>
+    <row r="18" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B18" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="56">
+        <v>5</v>
+      </c>
+      <c r="F18" s="54"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
+      <c r="N18" s="65"/>
+      <c r="O18" s="65"/>
+      <c r="P18" s="65"/>
+      <c r="Q18" s="65"/>
+      <c r="R18" s="65"/>
+      <c r="S18" s="65"/>
+      <c r="T18" s="65"/>
+    </row>
+    <row r="19" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="56">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B14" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="K14" s="6">
+      <c r="F19" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="65"/>
+      <c r="N19" s="65"/>
+      <c r="O19" s="65"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="65"/>
+      <c r="R19" s="65"/>
+      <c r="S19" s="65"/>
+      <c r="T19" s="65"/>
+    </row>
+    <row r="20" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="60">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B15" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="K15" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:20" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B16" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="20"/>
-      <c r="K16" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" s="6" customFormat="1" ht="27" customHeight="1" thickBot="1">
-      <c r="B17" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="K17" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B18" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="K18" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B19" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="K19" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B20" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="K20" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B21" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-    </row>
-    <row r="22" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B22" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="N22" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B23" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="J23" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B24" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="J24" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" s="6" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="B25" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="J25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K25" s="39"/>
-    </row>
-    <row r="26" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B26" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="J26" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B27" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-    </row>
-    <row r="28" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B28" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-    </row>
-    <row r="29" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B29" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-    </row>
-    <row r="30" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B30" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-    </row>
-    <row r="31" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B31" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-    </row>
-    <row r="32" spans="2:14" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B32" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="18"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="65"/>
+      <c r="N20" s="65"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="65"/>
+      <c r="S20" s="65"/>
+      <c r="T20" s="65"/>
+    </row>
+    <row r="21" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+    </row>
+    <row r="23" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+    </row>
+    <row r="24" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B24" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+    </row>
+    <row r="25" spans="2:20" s="6" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+      <c r="B25" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="K25" s="29"/>
+    </row>
+    <row r="26" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B26" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B27" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+    </row>
+    <row r="28" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B28" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+    </row>
+    <row r="29" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B29" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B30" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="2:20" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B32" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B33" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
+      <c r="B33" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C34" s="8"/>
-      <c r="E34" s="9"/>
-      <c r="G34" s="10"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="9"/>
+      <c r="H34" s="10"/>
     </row>
     <row r="35" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C35" s="8"/>
-      <c r="E35" s="9"/>
-      <c r="G35" s="10"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="9"/>
+      <c r="H35" s="10"/>
     </row>
     <row r="36" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C36" s="8"/>
-      <c r="E36" s="9"/>
-      <c r="G36" s="10"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="9"/>
+      <c r="H36" s="10"/>
     </row>
     <row r="37" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C37" s="50" t="s">
+      <c r="C37" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="51"/>
-      <c r="E37" s="9"/>
-      <c r="G37" s="10"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="9"/>
+      <c r="H37" s="10"/>
     </row>
     <row r="38" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C38" s="40">
+      <c r="C38" s="30">
         <v>3</v>
       </c>
-      <c r="D38" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="9"/>
-      <c r="G38" s="10"/>
+      <c r="D38" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="45"/>
+      <c r="F38" s="9"/>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C39" s="42">
-        <v>5</v>
-      </c>
-      <c r="D39" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="9"/>
-      <c r="G39" s="10"/>
+      <c r="C39" s="32">
+        <v>5</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="46"/>
+      <c r="F39" s="9"/>
+      <c r="H39" s="10"/>
     </row>
     <row r="40" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C40" s="44">
+      <c r="C40" s="34">
         <v>8</v>
       </c>
-      <c r="D40" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" s="9"/>
-      <c r="G40" s="10"/>
+      <c r="D40" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" s="47"/>
+      <c r="F40" s="9"/>
+      <c r="H40" s="10"/>
     </row>
     <row r="41" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C41" s="46">
+      <c r="C41" s="36">
         <v>13</v>
       </c>
-      <c r="D41" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="9"/>
-      <c r="G41" s="10"/>
+      <c r="D41" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="48"/>
+      <c r="F41" s="9"/>
+      <c r="H41" s="10"/>
     </row>
     <row r="42" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C42" s="48">
+      <c r="C42" s="38">
         <v>21</v>
       </c>
-      <c r="D42" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="9"/>
-      <c r="G42" s="10"/>
+      <c r="D42" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="49"/>
+      <c r="F42" s="9"/>
+      <c r="H42" s="10"/>
     </row>
     <row r="43" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C43" s="8"/>
-      <c r="E43" s="9"/>
-      <c r="G43" s="10"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="9"/>
+      <c r="H43" s="10"/>
     </row>
     <row r="44" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C44" s="8"/>
-      <c r="E44" s="9"/>
-      <c r="G44" s="10"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="9"/>
+      <c r="H44" s="10"/>
     </row>
     <row r="45" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C45" s="8"/>
-      <c r="E45" s="9"/>
-      <c r="G45" s="10"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="9"/>
+      <c r="H45" s="10"/>
     </row>
     <row r="46" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C46" s="8"/>
-      <c r="E46" s="9"/>
-      <c r="G46" s="10"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="9"/>
+      <c r="H46" s="10"/>
     </row>
     <row r="47" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C47" s="8"/>
-      <c r="E47" s="9"/>
-      <c r="G47" s="10"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="9"/>
+      <c r="H47" s="10"/>
     </row>
     <row r="48" spans="2:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C48" s="8"/>
-      <c r="E48" s="9"/>
-      <c r="G48" s="10"/>
-    </row>
-    <row r="49" spans="3:7" s="6" customFormat="1" ht="23.1" customHeight="1">
+      <c r="E48" s="63"/>
+      <c r="F48" s="9"/>
+      <c r="H48" s="10"/>
+    </row>
+    <row r="49" spans="3:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C49" s="8"/>
-      <c r="E49" s="9"/>
-      <c r="G49" s="10"/>
-    </row>
-    <row r="50" spans="3:7" s="6" customFormat="1" ht="23.1" customHeight="1">
+      <c r="E49" s="63"/>
+      <c r="F49" s="9"/>
+      <c r="H49" s="10"/>
+    </row>
+    <row r="50" spans="3:8" s="6" customFormat="1" ht="23.1" customHeight="1">
       <c r="C50" s="8"/>
-      <c r="E50" s="9"/>
-      <c r="G50" s="10"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="9"/>
+      <c r="H50" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B2:I2"/>
     <mergeCell ref="C37:D37"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="B5:E7 E8 C5:C8 B8:B9 B21:B33 B11:B17 B19">
+  <conditionalFormatting sqref="B5:E7 C5:C8 B8:B9 B21:B33 B11:B17 B19">
     <cfRule type="expression" dxfId="59" priority="69">
       <formula>$B5="Done!"</formula>
     </cfRule>
@@ -2446,7 +2696,7 @@
       <formula>$B5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
+  <conditionalFormatting sqref="D9:E9">
     <cfRule type="expression" dxfId="55" priority="61">
       <formula>$B9="Done!"</formula>
     </cfRule>
@@ -2460,7 +2710,7 @@
       <formula>$B9="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+  <conditionalFormatting sqref="D8:E8">
     <cfRule type="expression" dxfId="51" priority="53">
       <formula>$B8="Done!"</formula>
     </cfRule>
@@ -2488,7 +2738,7 @@
       <formula>$B9="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11 D14:D33">
+  <conditionalFormatting sqref="D11:E11 D14:E33">
     <cfRule type="expression" dxfId="43" priority="36">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
@@ -2533,7 +2783,7 @@
       <formula>$B10="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
+  <conditionalFormatting sqref="D10:E10">
     <cfRule type="expression" dxfId="30" priority="23">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
@@ -2592,7 +2842,7 @@
       <formula>$B20="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
+  <conditionalFormatting sqref="D12:E12">
     <cfRule type="expression" dxfId="13" priority="78">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
@@ -2623,7 +2873,7 @@
       <formula>#REF!="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
+  <conditionalFormatting sqref="D6:E6">
     <cfRule type="expression" dxfId="4" priority="118">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
@@ -2641,12 +2891,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B33 E5:E33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B33" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C4" location="Dados!A1" display="Artefato de Referência (XX#R)"/>
+    <hyperlink ref="C4" location="Dados!A1" display="Artefato de Referência (XX#R)" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -2655,7 +2905,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>